<commit_message>
final_sim: Implemented burn maneuvers files into the simulator.  z value of satellites is nonzero when a burn maneuver occurs.
</commit_message>
<xml_diff>
--- a/1_final-sim/neural_body/sim_configs/TestConfig.xlsx
+++ b/1_final-sim/neural_body/sim_configs/TestConfig.xlsx
@@ -1,18 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\craig\Documents\Git\neural-body\1_final-sim\neural_body\sim_configs\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6919C285-4C4B-4F80-990C-63728642C685}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="Sheet2" sheetId="2" r:id="rId5"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="10">
   <si>
     <t>Name</t>
   </si>
@@ -23,15 +32,6 @@
     <t>Altitude</t>
   </si>
   <si>
-    <t>VXStart</t>
-  </si>
-  <si>
-    <t>VYStart</t>
-  </si>
-  <si>
-    <t>VZStart</t>
-  </si>
-  <si>
     <t>MStart</t>
   </si>
   <si>
@@ -48,66 +48,74 @@
   </si>
   <si>
     <t>Probe II</t>
+  </si>
+  <si>
+    <t>StartSpeed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
-    <font/>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -297,20 +305,25 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -321,89 +334,80 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="2" t="s">
+      <c r="B2" s="2">
+        <v>800</v>
+      </c>
+      <c r="C2" s="2">
+        <v>500000</v>
+      </c>
+      <c r="D2" s="1">
+        <v>20000</v>
+      </c>
+      <c r="E2" s="2">
         <v>10</v>
       </c>
-      <c r="B2" s="2">
-        <v>800.0</v>
-      </c>
-      <c r="C2" s="2">
-        <v>500000.0</v>
-      </c>
-      <c r="D2" s="1">
-        <v>20000.0</v>
-      </c>
-      <c r="E2" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="F2" s="1">
-        <v>0.0</v>
+      <c r="F2" s="2">
+        <v>0</v>
       </c>
       <c r="G2" s="2">
-        <v>10.0</v>
-      </c>
-      <c r="H2" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="I2" s="2">
-        <v>-1500.0</v>
-      </c>
-      <c r="J2" s="1">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="3">
+        <v>-1500</v>
+      </c>
+      <c r="H2" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="E3" s="2">
+        <v>25</v>
+      </c>
+      <c r="F3" s="2">
+        <v>-250</v>
+      </c>
       <c r="G3" s="2">
-        <v>25.0</v>
-      </c>
-      <c r="H3" s="2">
-        <v>-250.0</v>
-      </c>
-      <c r="I3" s="2">
-        <v>-2500.0</v>
-      </c>
-      <c r="J3" s="1">
-        <v>0.0</v>
+        <v>-2500</v>
+      </c>
+      <c r="H3" s="1">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -414,74 +418,62 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="B2" s="1">
-        <v>400.0</v>
+        <v>400</v>
       </c>
       <c r="C2" s="1">
-        <v>300000.0</v>
+        <v>300000</v>
       </c>
       <c r="D2" s="1">
-        <v>15000.0</v>
-      </c>
-      <c r="E2" s="1">
-        <v>0.0</v>
+        <v>15000</v>
+      </c>
+      <c r="E2" s="2">
+        <v>10</v>
       </c>
       <c r="F2" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="G2" s="2">
-        <v>10.0</v>
+        <v>0</v>
+      </c>
+      <c r="G2" s="1">
+        <v>2000</v>
       </c>
       <c r="H2" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="I2" s="1">
-        <v>2000.0</v>
-      </c>
-      <c r="J2" s="1">
-        <v>100.0</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="G3" s="2">
-        <v>25.0</v>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="E3" s="2">
+        <v>25</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3" s="1">
+        <v>-1000</v>
       </c>
       <c r="H3" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="I3" s="1">
-        <v>-1000.0</v>
-      </c>
-      <c r="J3" s="1">
-        <v>-100.0</v>
+        <v>-100</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
final_sim:  Fixed reading of config files without maneuvers and made copy of old config.  Using config without maneuvers until new neural net is integrated.
</commit_message>
<xml_diff>
--- a/1_final-sim/neural_body/sim_configs/TestConfig.xlsx
+++ b/1_final-sim/neural_body/sim_configs/TestConfig.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\craig\Documents\Git\neural-body\1_final-sim\neural_body\sim_configs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6919C285-4C4B-4F80-990C-63728642C685}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CB279B5-B929-491F-AFED-F8D379CD9551}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -317,8 +317,8 @@
   </sheetPr>
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -354,40 +354,24 @@
         <v>7</v>
       </c>
       <c r="B2" s="2">
-        <v>800</v>
+        <v>3000</v>
       </c>
       <c r="C2" s="2">
-        <v>500000</v>
+        <v>5000000</v>
       </c>
       <c r="D2" s="1">
-        <v>20000</v>
-      </c>
-      <c r="E2" s="2">
-        <v>10</v>
-      </c>
-      <c r="F2" s="2">
-        <v>0</v>
-      </c>
-      <c r="G2" s="2">
-        <v>-1500</v>
-      </c>
-      <c r="H2" s="1">
-        <v>0</v>
-      </c>
+        <v>12000</v>
+      </c>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="1"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="E3" s="2">
-        <v>25</v>
-      </c>
-      <c r="F3" s="2">
-        <v>-250</v>
-      </c>
-      <c r="G3" s="2">
-        <v>-2500</v>
-      </c>
-      <c r="H3" s="1">
-        <v>0</v>
-      </c>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -401,8 +385,8 @@
   </sheetPr>
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -438,40 +422,24 @@
         <v>8</v>
       </c>
       <c r="B2" s="1">
-        <v>400</v>
+        <v>4000</v>
       </c>
       <c r="C2" s="1">
-        <v>300000</v>
+        <v>3000000</v>
       </c>
       <c r="D2" s="1">
-        <v>15000</v>
-      </c>
-      <c r="E2" s="2">
-        <v>10</v>
-      </c>
-      <c r="F2" s="1">
-        <v>0</v>
-      </c>
-      <c r="G2" s="1">
-        <v>2000</v>
-      </c>
-      <c r="H2" s="1">
-        <v>100</v>
-      </c>
+        <v>13000</v>
+      </c>
+      <c r="E2" s="2"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="E3" s="2">
-        <v>25</v>
-      </c>
-      <c r="F3" s="1">
-        <v>0</v>
-      </c>
-      <c r="G3" s="1">
-        <v>-1000</v>
-      </c>
-      <c r="H3" s="1">
-        <v>-100</v>
-      </c>
+      <c r="E3" s="2"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
final_sim: Catch orbits now that exceed large values over 10^25
</commit_message>
<xml_diff>
--- a/1_final-sim/neural_body/sim_configs/TestConfig.xlsx
+++ b/1_final-sim/neural_body/sim_configs/TestConfig.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\craig\Documents\Git\neural-body\1_final-sim\neural_body\sim_configs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CB279B5-B929-491F-AFED-F8D379CD9551}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32A005A0-2380-439D-8C79-FBCB21A8818F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -318,7 +318,7 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -362,16 +362,32 @@
       <c r="D2" s="1">
         <v>12000</v>
       </c>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="1"/>
+      <c r="E2" s="2">
+        <v>10</v>
+      </c>
+      <c r="F2" s="2">
+        <v>-1</v>
+      </c>
+      <c r="G2" s="2">
+        <v>1</v>
+      </c>
+      <c r="H2" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="1"/>
+      <c r="E3" s="2">
+        <v>25</v>
+      </c>
+      <c r="F3" s="2">
+        <v>2</v>
+      </c>
+      <c r="G3" s="2">
+        <v>2</v>
+      </c>
+      <c r="H3" s="1">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -386,7 +402,7 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:H4"/>
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -428,18 +444,34 @@
         <v>3000000</v>
       </c>
       <c r="D2" s="1">
-        <v>13000</v>
-      </c>
-      <c r="E2" s="2"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
+        <v>17000</v>
+      </c>
+      <c r="E2" s="2">
+        <v>10</v>
+      </c>
+      <c r="F2" s="1">
+        <v>1</v>
+      </c>
+      <c r="G2" s="1">
+        <v>-1</v>
+      </c>
+      <c r="H2" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="E3" s="2"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
+      <c r="E3" s="2">
+        <v>25</v>
+      </c>
+      <c r="F3" s="1">
+        <v>1</v>
+      </c>
+      <c r="G3" s="1">
+        <v>1</v>
+      </c>
+      <c r="H3" s="1">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
final_sim:  Added capability to choose whether or not to use the neural net in the config file in addition to the satellite tabs.
</commit_message>
<xml_diff>
--- a/1_final-sim/neural_body/sim_configs/TestConfig.xlsx
+++ b/1_final-sim/neural_body/sim_configs/TestConfig.xlsx
@@ -8,20 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\craig\Documents\Git\neural-body\1_final-sim\neural_body\sim_configs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32A005A0-2380-439D-8C79-FBCB21A8818F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCE99678-A384-41D5-8FDA-01AC808E25E9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="SimConfig" sheetId="3" r:id="rId1"/>
+    <sheet name="Sat1" sheetId="1" r:id="rId2"/>
+    <sheet name="Sat2" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="12">
   <si>
     <t>Name</t>
   </si>
@@ -51,6 +52,12 @@
   </si>
   <si>
     <t>StartSpeed</t>
+  </si>
+  <si>
+    <t>UseNeuralNet</t>
+  </si>
+  <si>
+    <t>no</t>
   </si>
 </sst>
 </file>
@@ -311,6 +318,34 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF846D29-C8D2-4A70-A77B-6EE37888FC0B}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -394,15 +429,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
final_sim:  Added file prompt and error checking for new sim config to grav2.  Should display error window if incompatible config file.
</commit_message>
<xml_diff>
--- a/1_final-sim/neural_body/sim_configs/TestConfig.xlsx
+++ b/1_final-sim/neural_body/sim_configs/TestConfig.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\craig\Documents\Git\neural-body\1_final-sim\neural_body\sim_configs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCE99678-A384-41D5-8FDA-01AC808E25E9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B307C487-529F-4416-BA93-1AC164BA4DFC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -322,7 +322,7 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>